<commit_message>
untabify and some cleanup
</commit_message>
<xml_diff>
--- a/HILLookupsAndTestResults.xlsx
+++ b/HILLookupsAndTestResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarah\Documents\Spring2017\EE445M\HILRacecarTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6891C93B-3763-4180-909F-071419A13270}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C0FB39-F0D1-478D-A3C4-999986B26B8F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="10060" firstSheet="5" activeTab="8" xr2:uid="{43983ABA-C9D5-414E-B198-F3BE803227D6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="23">
   <si>
     <t>mm</t>
   </si>
@@ -149,10 +149,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,6 +842,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-7BDD-48AD-86A9-4DC1DAD04B5C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:xVal>
             <c:numRef>
@@ -2811,19 +2816,12 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Demo!$B$43</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1500</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:f>Demo!#REF!</c:f>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demo!$C$43</c:f>
+              <c:f>Demo!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -28854,11 +28852,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
@@ -29817,11 +29815,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
@@ -31034,11 +31032,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
@@ -31719,11 +31717,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
@@ -32652,10 +32650,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF8FDF7D-F6CA-47C3-B261-ADF4D78B9A23}">
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32670,11 +32668,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
@@ -33412,7 +33410,7 @@
         <v>1298</v>
       </c>
       <c r="D56">
-        <v>4294966516</v>
+        <v>1112</v>
       </c>
       <c r="E56">
         <v>360</v>
@@ -33444,37 +33442,37 @@
         <v>14</v>
       </c>
       <c r="B57">
-        <v>1848</v>
+        <v>1926</v>
       </c>
       <c r="C57">
-        <v>1298</v>
+        <v>1409</v>
       </c>
       <c r="D57">
-        <v>4294966516</v>
+        <v>1112</v>
       </c>
       <c r="E57">
         <v>330</v>
       </c>
       <c r="F57">
-        <v>1152</v>
+        <v>1074</v>
       </c>
       <c r="G57">
-        <v>202</v>
+        <v>91</v>
       </c>
       <c r="H57" t="s">
         <v>5</v>
       </c>
       <c r="I57">
-        <v>202</v>
+        <v>91</v>
       </c>
       <c r="J57" t="s">
         <v>5</v>
       </c>
       <c r="K57">
-        <v>1192</v>
+        <v>351</v>
       </c>
       <c r="L57">
-        <v>1192</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">
@@ -33482,10 +33480,10 @@
         <v>15</v>
       </c>
       <c r="B58">
-        <v>1781</v>
+        <v>2022</v>
       </c>
       <c r="C58">
-        <v>1337</v>
+        <v>1354</v>
       </c>
       <c r="D58">
         <v>1112</v>
@@ -33494,25 +33492,25 @@
         <v>300</v>
       </c>
       <c r="F58">
-        <v>1407</v>
+        <v>1129</v>
       </c>
       <c r="G58">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="H58" t="s">
         <v>5</v>
       </c>
       <c r="I58">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="J58" t="s">
         <v>5</v>
       </c>
       <c r="K58">
-        <v>1261</v>
+        <v>1012</v>
       </c>
       <c r="L58">
-        <v>1183</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
@@ -33520,10 +33518,10 @@
         <v>16</v>
       </c>
       <c r="B59">
-        <v>1836</v>
+        <v>2077</v>
       </c>
       <c r="C59">
-        <v>1241</v>
+        <v>1258</v>
       </c>
       <c r="D59">
         <v>1112</v>
@@ -33532,25 +33530,25 @@
         <v>270</v>
       </c>
       <c r="F59">
-        <v>855</v>
+        <v>874</v>
       </c>
       <c r="G59">
-        <v>517</v>
+        <v>482</v>
       </c>
       <c r="H59">
-        <v>964</v>
+        <v>1243</v>
       </c>
       <c r="I59">
-        <v>517</v>
+        <v>482</v>
       </c>
       <c r="J59">
-        <v>964</v>
+        <v>1243</v>
       </c>
       <c r="K59">
-        <v>1047</v>
+        <v>1071</v>
       </c>
       <c r="L59">
-        <v>766</v>
+        <v>784</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
@@ -33558,10 +33556,10 @@
         <v>17</v>
       </c>
       <c r="B60">
-        <v>1836</v>
+        <v>2077</v>
       </c>
       <c r="C60">
-        <v>1130</v>
+        <v>1147</v>
       </c>
       <c r="D60">
         <v>1112</v>
@@ -33569,23 +33567,23 @@
       <c r="E60">
         <v>270</v>
       </c>
-      <c r="F60" t="s">
-        <v>5</v>
+      <c r="F60">
+        <v>647</v>
       </c>
       <c r="G60">
-        <v>1164</v>
+        <v>923</v>
       </c>
       <c r="H60">
-        <v>836</v>
+        <v>1077</v>
       </c>
       <c r="I60">
-        <v>1164</v>
+        <v>923</v>
       </c>
       <c r="J60">
-        <v>836</v>
+        <v>1077</v>
       </c>
       <c r="K60">
-        <v>652</v>
+        <v>669</v>
       </c>
       <c r="L60" t="s">
         <v>5</v>
@@ -33596,10 +33594,10 @@
         <v>18</v>
       </c>
       <c r="B61">
-        <v>1836</v>
+        <v>2077</v>
       </c>
       <c r="C61">
-        <v>1019</v>
+        <v>1036</v>
       </c>
       <c r="D61">
         <v>1112</v>
@@ -33607,23 +33605,23 @@
       <c r="E61">
         <v>270</v>
       </c>
-      <c r="F61" t="s">
-        <v>5</v>
+      <c r="F61">
+        <v>536</v>
       </c>
       <c r="G61">
-        <v>1164</v>
+        <v>923</v>
       </c>
       <c r="H61">
-        <v>836</v>
+        <v>1077</v>
       </c>
       <c r="I61">
-        <v>1164</v>
+        <v>923</v>
       </c>
       <c r="J61">
-        <v>836</v>
+        <v>1077</v>
       </c>
       <c r="K61">
-        <v>634</v>
+        <v>554</v>
       </c>
       <c r="L61" t="s">
         <v>5</v>
@@ -33634,10 +33632,10 @@
         <v>19</v>
       </c>
       <c r="B62">
-        <v>1836</v>
+        <v>2077</v>
       </c>
       <c r="C62">
-        <v>908</v>
+        <v>925</v>
       </c>
       <c r="D62">
         <v>1112</v>
@@ -33645,23 +33643,23 @@
       <c r="E62">
         <v>270</v>
       </c>
-      <c r="F62" t="s">
-        <v>5</v>
+      <c r="F62">
+        <v>425</v>
       </c>
       <c r="G62">
-        <v>1164</v>
+        <v>923</v>
       </c>
       <c r="H62">
-        <v>836</v>
+        <v>1077</v>
       </c>
       <c r="I62">
-        <v>1164</v>
+        <v>923</v>
       </c>
       <c r="J62">
-        <v>836</v>
+        <v>1077</v>
       </c>
       <c r="K62">
-        <v>634</v>
+        <v>439</v>
       </c>
       <c r="L62" t="s">
         <v>5</v>
@@ -33672,10 +33670,10 @@
         <v>20</v>
       </c>
       <c r="B63">
-        <v>1836</v>
+        <v>2077</v>
       </c>
       <c r="C63">
-        <v>797</v>
+        <v>814</v>
       </c>
       <c r="D63">
         <v>1112</v>
@@ -33683,23 +33681,23 @@
       <c r="E63">
         <v>270</v>
       </c>
-      <c r="F63" t="s">
-        <v>5</v>
+      <c r="F63">
+        <v>314</v>
       </c>
       <c r="G63">
-        <v>1164</v>
+        <v>923</v>
       </c>
       <c r="H63">
-        <v>836</v>
+        <v>1077</v>
       </c>
       <c r="I63">
-        <v>1164</v>
+        <v>923</v>
       </c>
       <c r="J63">
-        <v>836</v>
+        <v>1077</v>
       </c>
       <c r="K63">
-        <v>634</v>
+        <v>325</v>
       </c>
       <c r="L63" t="s">
         <v>5</v>
@@ -33710,10 +33708,10 @@
         <v>21</v>
       </c>
       <c r="B64">
-        <v>1836</v>
+        <v>2077</v>
       </c>
       <c r="C64">
-        <v>686</v>
+        <v>703</v>
       </c>
       <c r="D64">
         <v>1112</v>
@@ -33721,26 +33719,26 @@
       <c r="E64">
         <v>270</v>
       </c>
-      <c r="F64" t="s">
-        <v>5</v>
+      <c r="F64">
+        <v>203</v>
       </c>
       <c r="G64">
-        <v>1164</v>
+        <v>923</v>
       </c>
       <c r="H64">
-        <v>836</v>
+        <v>1077</v>
       </c>
       <c r="I64">
-        <v>1164</v>
+        <v>923</v>
       </c>
       <c r="J64">
-        <v>836</v>
+        <v>1077</v>
       </c>
       <c r="K64">
-        <v>634</v>
-      </c>
-      <c r="L64" t="s">
-        <v>5</v>
+        <v>210</v>
+      </c>
+      <c r="L64">
+        <v>210</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.35">
@@ -33748,10 +33746,10 @@
         <v>22</v>
       </c>
       <c r="B65">
-        <v>1836</v>
+        <v>2077</v>
       </c>
       <c r="C65">
-        <v>575</v>
+        <v>592</v>
       </c>
       <c r="D65">
         <v>1112</v>
@@ -33759,292 +33757,26 @@
       <c r="E65">
         <v>270</v>
       </c>
-      <c r="F65" t="s">
-        <v>5</v>
+      <c r="F65">
+        <v>92</v>
       </c>
       <c r="G65">
-        <v>1164</v>
+        <v>923</v>
       </c>
       <c r="H65">
-        <v>836</v>
+        <v>1077</v>
       </c>
       <c r="I65">
-        <v>1164</v>
+        <v>923</v>
       </c>
       <c r="J65">
-        <v>836</v>
-      </c>
-      <c r="K65" t="s">
-        <v>5</v>
-      </c>
-      <c r="L65" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A66">
-        <v>23</v>
-      </c>
-      <c r="B66">
-        <v>1836</v>
-      </c>
-      <c r="C66">
-        <v>464</v>
-      </c>
-      <c r="D66">
-        <v>1112</v>
-      </c>
-      <c r="E66">
-        <v>240</v>
-      </c>
-      <c r="F66" t="s">
-        <v>5</v>
-      </c>
-      <c r="G66">
-        <v>164</v>
-      </c>
-      <c r="H66">
-        <v>836</v>
-      </c>
-      <c r="I66">
-        <v>164</v>
-      </c>
-      <c r="J66">
-        <v>836</v>
-      </c>
-      <c r="K66" t="s">
-        <v>5</v>
-      </c>
-      <c r="L66" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A67">
-        <v>24</v>
-      </c>
-      <c r="B67">
-        <v>1781</v>
-      </c>
-      <c r="C67">
-        <v>368</v>
-      </c>
-      <c r="D67">
-        <v>1112</v>
-      </c>
-      <c r="E67">
-        <v>210</v>
-      </c>
-      <c r="F67" t="s">
-        <v>5</v>
-      </c>
-      <c r="G67">
-        <v>253</v>
-      </c>
-      <c r="H67">
-        <v>901</v>
-      </c>
-      <c r="I67">
-        <v>253</v>
-      </c>
-      <c r="J67">
-        <v>901</v>
-      </c>
-      <c r="K67" t="s">
-        <v>5</v>
-      </c>
-      <c r="L67" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A68">
-        <v>25</v>
-      </c>
-      <c r="B68">
-        <v>1685</v>
-      </c>
-      <c r="C68">
-        <v>313</v>
-      </c>
-      <c r="D68">
-        <v>1112</v>
-      </c>
-      <c r="E68">
-        <v>210</v>
-      </c>
-      <c r="F68" t="s">
-        <v>5</v>
-      </c>
-      <c r="G68" t="s">
-        <v>5</v>
-      </c>
-      <c r="H68">
-        <v>1369</v>
-      </c>
-      <c r="I68" t="s">
-        <v>5</v>
-      </c>
-      <c r="J68">
-        <v>1369</v>
-      </c>
-      <c r="K68" t="s">
-        <v>5</v>
-      </c>
-      <c r="L68">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A69">
-        <v>26</v>
-      </c>
-      <c r="B69">
-        <v>1589</v>
-      </c>
-      <c r="C69">
-        <v>258</v>
-      </c>
-      <c r="D69">
-        <v>1112</v>
-      </c>
-      <c r="E69">
-        <v>210</v>
-      </c>
-      <c r="F69" t="s">
-        <v>5</v>
-      </c>
-      <c r="G69" t="s">
-        <v>5</v>
-      </c>
-      <c r="H69">
-        <v>1177</v>
-      </c>
-      <c r="I69" t="s">
-        <v>5</v>
-      </c>
-      <c r="J69">
-        <v>1177</v>
-      </c>
-      <c r="K69" t="s">
-        <v>5</v>
-      </c>
-      <c r="L69">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A70">
-        <v>27</v>
-      </c>
-      <c r="B70">
-        <v>1493</v>
-      </c>
-      <c r="C70">
-        <v>203</v>
-      </c>
-      <c r="D70">
-        <v>1112</v>
-      </c>
-      <c r="E70">
-        <v>210</v>
-      </c>
-      <c r="F70" t="s">
-        <v>5</v>
-      </c>
-      <c r="G70" t="s">
-        <v>5</v>
-      </c>
-      <c r="H70">
-        <v>985</v>
-      </c>
-      <c r="I70" t="s">
-        <v>5</v>
-      </c>
-      <c r="J70">
-        <v>985</v>
-      </c>
-      <c r="K70" t="s">
-        <v>5</v>
-      </c>
-      <c r="L70">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A71">
-        <v>28</v>
-      </c>
-      <c r="B71">
-        <v>1397</v>
-      </c>
-      <c r="C71">
-        <v>148</v>
-      </c>
-      <c r="D71">
-        <v>1112</v>
-      </c>
-      <c r="E71">
-        <v>210</v>
-      </c>
-      <c r="F71" t="s">
-        <v>5</v>
-      </c>
-      <c r="G71" t="s">
-        <v>5</v>
-      </c>
-      <c r="H71">
-        <v>793</v>
-      </c>
-      <c r="I71" t="s">
-        <v>5</v>
-      </c>
-      <c r="J71">
-        <v>793</v>
-      </c>
-      <c r="K71" t="s">
-        <v>5</v>
-      </c>
-      <c r="L71">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A72">
-        <v>29</v>
-      </c>
-      <c r="B72">
-        <v>1301</v>
-      </c>
-      <c r="C72">
-        <v>93</v>
-      </c>
-      <c r="D72">
-        <v>1112</v>
-      </c>
-      <c r="E72">
-        <v>240</v>
-      </c>
-      <c r="F72" t="s">
-        <v>5</v>
-      </c>
-      <c r="G72" t="s">
-        <v>5</v>
-      </c>
-      <c r="H72">
-        <v>601</v>
-      </c>
-      <c r="I72" t="s">
-        <v>5</v>
-      </c>
-      <c r="J72">
-        <v>601</v>
-      </c>
-      <c r="K72" t="s">
-        <v>5</v>
-      </c>
-      <c r="L72">
-        <v>311</v>
+        <v>1077</v>
+      </c>
+      <c r="K65">
+        <v>95</v>
+      </c>
+      <c r="L65">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add report and detabify
</commit_message>
<xml_diff>
--- a/HILLookupsAndTestResults.xlsx
+++ b/HILLookupsAndTestResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarah\Documents\Spring2017\EE445M\HILRacecarTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C0FB39-F0D1-478D-A3C4-999986B26B8F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD83F3AE-D69C-4A71-BD23-7AA156C08167}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="10060" firstSheet="5" activeTab="8" xr2:uid="{43983ABA-C9D5-414E-B198-F3BE803227D6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2930" windowHeight="8680" firstSheet="4" activeTab="7" xr2:uid="{43983ABA-C9D5-414E-B198-F3BE803227D6}"/>
   </bookViews>
   <sheets>
     <sheet name="SIN" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="23">
   <si>
     <t>mm</t>
   </si>
@@ -205,7 +205,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Simulation</a:t>
+              <a:t>Straight Track Simulation</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -314,7 +314,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3000</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -767,7 +767,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Simulation</a:t>
+              <a:t>Wide Turn Simulation</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -900,7 +900,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3000</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0</c:v>
@@ -1963,7 +1963,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Simulation</a:t>
+              <a:t>Tight Turn Simulation</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -2096,7 +2096,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3000</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0</c:v>
@@ -28837,7 +28837,7 @@
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28930,7 +28930,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B13">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -29800,7 +29800,7 @@
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29957,7 +29957,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B25">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -31016,7 +31016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E9645EE-321B-4160-A029-A8959ADAB7D0}">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A54" sqref="A54:L67"/>
     </sheetView>
   </sheetViews>
@@ -31701,8 +31701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B226846-4AEE-4091-BED0-7195DEAE37D7}">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -31859,7 +31859,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B25">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -32650,10 +32650,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF8FDF7D-F6CA-47C3-B261-ADF4D78B9A23}">
-  <dimension ref="A1:L65"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32905,880 +32905,6 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A43">
-        <v>0</v>
-      </c>
-      <c r="B43">
-        <v>1500</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43">
-        <v>1112</v>
-      </c>
-      <c r="E43">
-        <v>90</v>
-      </c>
-      <c r="F43">
-        <v>1499</v>
-      </c>
-      <c r="G43">
-        <v>500</v>
-      </c>
-      <c r="H43">
-        <v>500</v>
-      </c>
-      <c r="I43">
-        <v>500</v>
-      </c>
-      <c r="J43">
-        <v>500</v>
-      </c>
-      <c r="K43" t="s">
-        <v>5</v>
-      </c>
-      <c r="L43" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A44">
-        <v>1</v>
-      </c>
-      <c r="B44">
-        <v>1500</v>
-      </c>
-      <c r="C44">
-        <v>112</v>
-      </c>
-      <c r="D44">
-        <v>1112</v>
-      </c>
-      <c r="E44">
-        <v>90</v>
-      </c>
-      <c r="F44">
-        <v>1388</v>
-      </c>
-      <c r="G44">
-        <v>500</v>
-      </c>
-      <c r="H44">
-        <v>500</v>
-      </c>
-      <c r="I44">
-        <v>500</v>
-      </c>
-      <c r="J44">
-        <v>500</v>
-      </c>
-      <c r="K44">
-        <v>1436</v>
-      </c>
-      <c r="L44">
-        <v>1436</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A45">
-        <v>2</v>
-      </c>
-      <c r="B45">
-        <v>1500</v>
-      </c>
-      <c r="C45">
-        <v>223</v>
-      </c>
-      <c r="D45">
-        <v>1112</v>
-      </c>
-      <c r="E45">
-        <v>90</v>
-      </c>
-      <c r="F45">
-        <v>1277</v>
-      </c>
-      <c r="G45">
-        <v>500</v>
-      </c>
-      <c r="H45">
-        <v>500</v>
-      </c>
-      <c r="I45">
-        <v>500</v>
-      </c>
-      <c r="J45">
-        <v>500</v>
-      </c>
-      <c r="K45">
-        <v>1322</v>
-      </c>
-      <c r="L45">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A46">
-        <v>3</v>
-      </c>
-      <c r="B46">
-        <v>1500</v>
-      </c>
-      <c r="C46">
-        <v>334</v>
-      </c>
-      <c r="D46">
-        <v>1112</v>
-      </c>
-      <c r="E46">
-        <v>90</v>
-      </c>
-      <c r="F46">
-        <v>1166</v>
-      </c>
-      <c r="G46">
-        <v>500</v>
-      </c>
-      <c r="H46">
-        <v>500</v>
-      </c>
-      <c r="I46">
-        <v>500</v>
-      </c>
-      <c r="J46">
-        <v>500</v>
-      </c>
-      <c r="K46">
-        <v>1207</v>
-      </c>
-      <c r="L46">
-        <v>1207</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A47">
-        <v>4</v>
-      </c>
-      <c r="B47">
-        <v>1500</v>
-      </c>
-      <c r="C47">
-        <v>445</v>
-      </c>
-      <c r="D47">
-        <v>1112</v>
-      </c>
-      <c r="E47">
-        <v>90</v>
-      </c>
-      <c r="F47">
-        <v>1055</v>
-      </c>
-      <c r="G47">
-        <v>500</v>
-      </c>
-      <c r="H47">
-        <v>500</v>
-      </c>
-      <c r="I47">
-        <v>500</v>
-      </c>
-      <c r="J47">
-        <v>500</v>
-      </c>
-      <c r="K47">
-        <v>1092</v>
-      </c>
-      <c r="L47">
-        <v>1092</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A48">
-        <v>5</v>
-      </c>
-      <c r="B48">
-        <v>1500</v>
-      </c>
-      <c r="C48">
-        <v>556</v>
-      </c>
-      <c r="D48">
-        <v>1112</v>
-      </c>
-      <c r="E48">
-        <v>60</v>
-      </c>
-      <c r="F48">
-        <v>944</v>
-      </c>
-      <c r="G48">
-        <v>500</v>
-      </c>
-      <c r="H48">
-        <v>1500</v>
-      </c>
-      <c r="I48">
-        <v>500</v>
-      </c>
-      <c r="J48">
-        <v>1500</v>
-      </c>
-      <c r="K48">
-        <v>977</v>
-      </c>
-      <c r="L48">
-        <v>977</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A49">
-        <v>6</v>
-      </c>
-      <c r="B49">
-        <v>1555</v>
-      </c>
-      <c r="C49">
-        <v>652</v>
-      </c>
-      <c r="D49">
-        <v>1112</v>
-      </c>
-      <c r="E49">
-        <v>90</v>
-      </c>
-      <c r="F49">
-        <v>978</v>
-      </c>
-      <c r="G49">
-        <v>640</v>
-      </c>
-      <c r="H49">
-        <v>513</v>
-      </c>
-      <c r="I49">
-        <v>640</v>
-      </c>
-      <c r="J49">
-        <v>513</v>
-      </c>
-      <c r="K49">
-        <v>877</v>
-      </c>
-      <c r="L49">
-        <v>1199</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A50">
-        <v>7</v>
-      </c>
-      <c r="B50">
-        <v>1555</v>
-      </c>
-      <c r="C50">
-        <v>763</v>
-      </c>
-      <c r="D50">
-        <v>1112</v>
-      </c>
-      <c r="E50">
-        <v>60</v>
-      </c>
-      <c r="F50">
-        <v>737</v>
-      </c>
-      <c r="G50">
-        <v>555</v>
-      </c>
-      <c r="H50">
-        <v>1445</v>
-      </c>
-      <c r="I50">
-        <v>555</v>
-      </c>
-      <c r="J50">
-        <v>1445</v>
-      </c>
-      <c r="K50">
-        <v>763</v>
-      </c>
-      <c r="L50">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A51">
-        <v>8</v>
-      </c>
-      <c r="B51">
-        <v>1610</v>
-      </c>
-      <c r="C51">
-        <v>859</v>
-      </c>
-      <c r="D51">
-        <v>1112</v>
-      </c>
-      <c r="E51">
-        <v>60</v>
-      </c>
-      <c r="F51">
-        <v>739</v>
-      </c>
-      <c r="G51">
-        <v>703</v>
-      </c>
-      <c r="H51">
-        <v>716</v>
-      </c>
-      <c r="I51">
-        <v>703</v>
-      </c>
-      <c r="J51">
-        <v>716</v>
-      </c>
-      <c r="K51">
-        <v>663</v>
-      </c>
-      <c r="L51">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A52">
-        <v>9</v>
-      </c>
-      <c r="B52">
-        <v>1665</v>
-      </c>
-      <c r="C52">
-        <v>955</v>
-      </c>
-      <c r="D52">
-        <v>1112</v>
-      </c>
-      <c r="E52">
-        <v>60</v>
-      </c>
-      <c r="F52">
-        <v>628</v>
-      </c>
-      <c r="G52">
-        <v>767</v>
-      </c>
-      <c r="H52">
-        <v>909</v>
-      </c>
-      <c r="I52">
-        <v>767</v>
-      </c>
-      <c r="J52">
-        <v>909</v>
-      </c>
-      <c r="K52">
-        <v>563</v>
-      </c>
-      <c r="L52">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A53">
-        <v>10</v>
-      </c>
-      <c r="B53">
-        <v>1720</v>
-      </c>
-      <c r="C53">
-        <v>1051</v>
-      </c>
-      <c r="D53">
-        <v>1112</v>
-      </c>
-      <c r="E53">
-        <v>60</v>
-      </c>
-      <c r="F53">
-        <v>518</v>
-      </c>
-      <c r="G53">
-        <v>831</v>
-      </c>
-      <c r="H53">
-        <v>1101</v>
-      </c>
-      <c r="I53">
-        <v>831</v>
-      </c>
-      <c r="J53">
-        <v>1101</v>
-      </c>
-      <c r="K53">
-        <v>464</v>
-      </c>
-      <c r="L53">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A54">
-        <v>11</v>
-      </c>
-      <c r="B54">
-        <v>1775</v>
-      </c>
-      <c r="C54">
-        <v>1147</v>
-      </c>
-      <c r="D54">
-        <v>1112</v>
-      </c>
-      <c r="E54">
-        <v>60</v>
-      </c>
-      <c r="F54">
-        <v>407</v>
-      </c>
-      <c r="G54">
-        <v>707</v>
-      </c>
-      <c r="H54">
-        <v>1294</v>
-      </c>
-      <c r="I54">
-        <v>707</v>
-      </c>
-      <c r="J54">
-        <v>1294</v>
-      </c>
-      <c r="K54">
-        <v>365</v>
-      </c>
-      <c r="L54">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A55">
-        <v>12</v>
-      </c>
-      <c r="B55">
-        <v>1830</v>
-      </c>
-      <c r="C55">
-        <v>1243</v>
-      </c>
-      <c r="D55">
-        <v>1112</v>
-      </c>
-      <c r="E55">
-        <v>30</v>
-      </c>
-      <c r="F55">
-        <v>296</v>
-      </c>
-      <c r="G55">
-        <v>515</v>
-      </c>
-      <c r="H55">
-        <v>1351</v>
-      </c>
-      <c r="I55">
-        <v>515</v>
-      </c>
-      <c r="J55">
-        <v>1351</v>
-      </c>
-      <c r="K55">
-        <v>265</v>
-      </c>
-      <c r="L55">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A56">
-        <v>13</v>
-      </c>
-      <c r="B56">
-        <v>1926</v>
-      </c>
-      <c r="C56">
-        <v>1298</v>
-      </c>
-      <c r="D56">
-        <v>1112</v>
-      </c>
-      <c r="E56">
-        <v>360</v>
-      </c>
-      <c r="F56">
-        <v>403</v>
-      </c>
-      <c r="G56">
-        <v>233</v>
-      </c>
-      <c r="H56">
-        <v>921</v>
-      </c>
-      <c r="I56">
-        <v>233</v>
-      </c>
-      <c r="J56">
-        <v>921</v>
-      </c>
-      <c r="K56">
-        <v>285</v>
-      </c>
-      <c r="L56">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A57">
-        <v>14</v>
-      </c>
-      <c r="B57">
-        <v>1926</v>
-      </c>
-      <c r="C57">
-        <v>1409</v>
-      </c>
-      <c r="D57">
-        <v>1112</v>
-      </c>
-      <c r="E57">
-        <v>330</v>
-      </c>
-      <c r="F57">
-        <v>1074</v>
-      </c>
-      <c r="G57">
-        <v>91</v>
-      </c>
-      <c r="H57" t="s">
-        <v>5</v>
-      </c>
-      <c r="I57">
-        <v>91</v>
-      </c>
-      <c r="J57" t="s">
-        <v>5</v>
-      </c>
-      <c r="K57">
-        <v>351</v>
-      </c>
-      <c r="L57">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A58">
-        <v>15</v>
-      </c>
-      <c r="B58">
-        <v>2022</v>
-      </c>
-      <c r="C58">
-        <v>1354</v>
-      </c>
-      <c r="D58">
-        <v>1112</v>
-      </c>
-      <c r="E58">
-        <v>300</v>
-      </c>
-      <c r="F58">
-        <v>1129</v>
-      </c>
-      <c r="G58">
-        <v>168</v>
-      </c>
-      <c r="H58" t="s">
-        <v>5</v>
-      </c>
-      <c r="I58">
-        <v>168</v>
-      </c>
-      <c r="J58" t="s">
-        <v>5</v>
-      </c>
-      <c r="K58">
-        <v>1012</v>
-      </c>
-      <c r="L58">
-        <v>1207</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A59">
-        <v>16</v>
-      </c>
-      <c r="B59">
-        <v>2077</v>
-      </c>
-      <c r="C59">
-        <v>1258</v>
-      </c>
-      <c r="D59">
-        <v>1112</v>
-      </c>
-      <c r="E59">
-        <v>270</v>
-      </c>
-      <c r="F59">
-        <v>874</v>
-      </c>
-      <c r="G59">
-        <v>482</v>
-      </c>
-      <c r="H59">
-        <v>1243</v>
-      </c>
-      <c r="I59">
-        <v>482</v>
-      </c>
-      <c r="J59">
-        <v>1243</v>
-      </c>
-      <c r="K59">
-        <v>1071</v>
-      </c>
-      <c r="L59">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A60">
-        <v>17</v>
-      </c>
-      <c r="B60">
-        <v>2077</v>
-      </c>
-      <c r="C60">
-        <v>1147</v>
-      </c>
-      <c r="D60">
-        <v>1112</v>
-      </c>
-      <c r="E60">
-        <v>270</v>
-      </c>
-      <c r="F60">
-        <v>647</v>
-      </c>
-      <c r="G60">
-        <v>923</v>
-      </c>
-      <c r="H60">
-        <v>1077</v>
-      </c>
-      <c r="I60">
-        <v>923</v>
-      </c>
-      <c r="J60">
-        <v>1077</v>
-      </c>
-      <c r="K60">
-        <v>669</v>
-      </c>
-      <c r="L60" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A61">
-        <v>18</v>
-      </c>
-      <c r="B61">
-        <v>2077</v>
-      </c>
-      <c r="C61">
-        <v>1036</v>
-      </c>
-      <c r="D61">
-        <v>1112</v>
-      </c>
-      <c r="E61">
-        <v>270</v>
-      </c>
-      <c r="F61">
-        <v>536</v>
-      </c>
-      <c r="G61">
-        <v>923</v>
-      </c>
-      <c r="H61">
-        <v>1077</v>
-      </c>
-      <c r="I61">
-        <v>923</v>
-      </c>
-      <c r="J61">
-        <v>1077</v>
-      </c>
-      <c r="K61">
-        <v>554</v>
-      </c>
-      <c r="L61" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A62">
-        <v>19</v>
-      </c>
-      <c r="B62">
-        <v>2077</v>
-      </c>
-      <c r="C62">
-        <v>925</v>
-      </c>
-      <c r="D62">
-        <v>1112</v>
-      </c>
-      <c r="E62">
-        <v>270</v>
-      </c>
-      <c r="F62">
-        <v>425</v>
-      </c>
-      <c r="G62">
-        <v>923</v>
-      </c>
-      <c r="H62">
-        <v>1077</v>
-      </c>
-      <c r="I62">
-        <v>923</v>
-      </c>
-      <c r="J62">
-        <v>1077</v>
-      </c>
-      <c r="K62">
-        <v>439</v>
-      </c>
-      <c r="L62" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A63">
-        <v>20</v>
-      </c>
-      <c r="B63">
-        <v>2077</v>
-      </c>
-      <c r="C63">
-        <v>814</v>
-      </c>
-      <c r="D63">
-        <v>1112</v>
-      </c>
-      <c r="E63">
-        <v>270</v>
-      </c>
-      <c r="F63">
-        <v>314</v>
-      </c>
-      <c r="G63">
-        <v>923</v>
-      </c>
-      <c r="H63">
-        <v>1077</v>
-      </c>
-      <c r="I63">
-        <v>923</v>
-      </c>
-      <c r="J63">
-        <v>1077</v>
-      </c>
-      <c r="K63">
-        <v>325</v>
-      </c>
-      <c r="L63" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A64">
-        <v>21</v>
-      </c>
-      <c r="B64">
-        <v>2077</v>
-      </c>
-      <c r="C64">
-        <v>703</v>
-      </c>
-      <c r="D64">
-        <v>1112</v>
-      </c>
-      <c r="E64">
-        <v>270</v>
-      </c>
-      <c r="F64">
-        <v>203</v>
-      </c>
-      <c r="G64">
-        <v>923</v>
-      </c>
-      <c r="H64">
-        <v>1077</v>
-      </c>
-      <c r="I64">
-        <v>923</v>
-      </c>
-      <c r="J64">
-        <v>1077</v>
-      </c>
-      <c r="K64">
-        <v>210</v>
-      </c>
-      <c r="L64">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A65">
-        <v>22</v>
-      </c>
-      <c r="B65">
-        <v>2077</v>
-      </c>
-      <c r="C65">
-        <v>592</v>
-      </c>
-      <c r="D65">
-        <v>1112</v>
-      </c>
-      <c r="E65">
-        <v>270</v>
-      </c>
-      <c r="F65">
-        <v>92</v>
-      </c>
-      <c r="G65">
-        <v>923</v>
-      </c>
-      <c r="H65">
-        <v>1077</v>
-      </c>
-      <c r="I65">
-        <v>923</v>
-      </c>
-      <c r="J65">
-        <v>1077</v>
-      </c>
-      <c r="K65">
-        <v>95</v>
-      </c>
-      <c r="L65">
-        <v>95</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>

</xml_diff>